<commit_message>
Modified Absentees bug and consolidated output bug
</commit_message>
<xml_diff>
--- a/combined_output_new.xlsx
+++ b/combined_output_new.xlsx
@@ -16,35 +16,35 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="55">
   <si>
     <t>Course Code</t>
   </si>
   <si>
+    <t>DSPC604</t>
+  </si>
+  <si>
+    <t>DSPE605</t>
+  </si>
+  <si>
     <t>DSPC608</t>
   </si>
   <si>
+    <t>DSPC601</t>
+  </si>
+  <si>
+    <t>EEOE 606</t>
+  </si>
+  <si>
     <t>DSPC602</t>
   </si>
   <si>
+    <t>DSPE603</t>
+  </si>
+  <si>
     <t>DSPC607</t>
   </si>
   <si>
-    <t>DSPE603</t>
-  </si>
-  <si>
-    <t>DSPC604</t>
-  </si>
-  <si>
-    <t>DSPC601</t>
-  </si>
-  <si>
-    <t>EEOE 606</t>
-  </si>
-  <si>
-    <t>DSPE605</t>
-  </si>
-  <si>
     <t>Total Students</t>
   </si>
   <si>
@@ -57,13 +57,13 @@
     <t>Average Marks</t>
   </si>
   <si>
-    <t>Students Less than 16</t>
-  </si>
-  <si>
-    <t>Students Between 16 and 30</t>
-  </si>
-  <si>
-    <t>Students More than 30</t>
+    <t>Students Less than 40%</t>
+  </si>
+  <si>
+    <t>Students Between 40 %. and 75 %</t>
+  </si>
+  <si>
+    <t>Students More than 75%</t>
   </si>
   <si>
     <t>Roll No.</t>
@@ -78,94 +78,106 @@
     <t>Mohammed Azees M</t>
   </si>
   <si>
+    <t>Manuneethi S</t>
+  </si>
+  <si>
+    <t>Balaganapathi A</t>
+  </si>
+  <si>
     <t>Krishnakumar S</t>
   </si>
   <si>
-    <t>Manuneethi S</t>
-  </si>
-  <si>
     <t>MARIKANNAN P</t>
   </si>
   <si>
-    <t>Balaganapathi A</t>
-  </si>
-  <si>
     <t>SATHISHKUMAR N</t>
   </si>
   <si>
+    <t>Upanshu</t>
+  </si>
+  <si>
+    <t>JAISANKAR S</t>
+  </si>
+  <si>
+    <t>Sanjay S</t>
+  </si>
+  <si>
+    <t>DHINAKARAN R</t>
+  </si>
+  <si>
+    <t>Manoharan K</t>
+  </si>
+  <si>
     <t>Arulselvam C</t>
   </si>
   <si>
-    <t>Upanshu</t>
-  </si>
-  <si>
-    <t>JAISANKAR S</t>
-  </si>
-  <si>
     <t>Jaikrishnan V</t>
   </si>
   <si>
     <t>Aravind S</t>
   </si>
   <si>
+    <t>Hitesh Kumar K A</t>
+  </si>
+  <si>
+    <t>Naveena A</t>
+  </si>
+  <si>
+    <t>Jananika B</t>
+  </si>
+  <si>
+    <t>Sivaa Ganesh S</t>
+  </si>
+  <si>
     <t>Brijesh A</t>
   </si>
   <si>
+    <t>Ashik Jenly V L</t>
+  </si>
+  <si>
+    <t>Subhashini S</t>
+  </si>
+  <si>
     <t>Nithya Sri R</t>
   </si>
   <si>
+    <t>Preethiga S</t>
+  </si>
+  <si>
+    <t>Kalaivani S</t>
+  </si>
+  <si>
+    <t>AJAY S</t>
+  </si>
+  <si>
+    <t>Suji Shri B</t>
+  </si>
+  <si>
+    <t>Pradeep M</t>
+  </si>
+  <si>
+    <t>Gowtham R</t>
+  </si>
+  <si>
     <t>Kailashwaran R</t>
   </si>
   <si>
-    <t>Hitesh Kumar K A</t>
+    <t>Mohamed Suhail J</t>
+  </si>
+  <si>
+    <t>Krishnapriya K</t>
   </si>
   <si>
     <t>Deepakragavan J</t>
   </si>
   <si>
-    <t>Suji Shri B</t>
-  </si>
-  <si>
-    <t>Preethiga S</t>
-  </si>
-  <si>
-    <t>Subhashini S</t>
-  </si>
-  <si>
-    <t>Sivaa Ganesh S</t>
-  </si>
-  <si>
-    <t>Gowtham R</t>
-  </si>
-  <si>
-    <t>Bhuvanadurai M</t>
-  </si>
-  <si>
-    <t>Ashik Jenly V L</t>
-  </si>
-  <si>
-    <t>Krishnapriya K</t>
-  </si>
-  <si>
-    <t>Mohamed Suhail J</t>
-  </si>
-  <si>
-    <t>Pradeep M</t>
-  </si>
-  <si>
-    <t>Kalaivani S</t>
-  </si>
-  <si>
     <t>Guruprasath V</t>
   </si>
   <si>
-    <t>Naveena A</t>
+    <t>Varsha V</t>
   </si>
   <si>
     <t>Nawin B</t>
-  </si>
-  <si>
-    <t>Jananika B</t>
   </si>
   <si>
     <t>Srija D</t>
@@ -601,7 +613,7 @@
         <v>51</v>
       </c>
       <c r="D3">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E3">
         <v>51</v>
@@ -616,7 +628,7 @@
         <v>51</v>
       </c>
       <c r="I3">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -630,7 +642,7 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -645,7 +657,7 @@
         <v>0</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -653,28 +665,28 @@
         <v>12</v>
       </c>
       <c r="B5">
-        <v>12.88235294117647</v>
+        <v>12.88</v>
       </c>
       <c r="C5">
-        <v>19.03921568627451</v>
+        <v>19.04</v>
       </c>
       <c r="D5">
-        <v>6.84313725490196</v>
+        <v>7.12</v>
       </c>
       <c r="E5">
-        <v>26.84313725490196</v>
+        <v>26.84</v>
       </c>
       <c r="F5">
-        <v>22.2156862745098</v>
+        <v>22.22</v>
       </c>
       <c r="G5">
-        <v>19.88235294117647</v>
+        <v>19.88</v>
       </c>
       <c r="H5">
-        <v>27.23529411764706</v>
+        <v>27.24</v>
       </c>
       <c r="I5">
-        <v>11.01960784313725</v>
+        <v>11.71</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -688,7 +700,7 @@
         <v>15</v>
       </c>
       <c r="D6">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E6">
         <v>6</v>
@@ -703,7 +715,7 @@
         <v>7</v>
       </c>
       <c r="I6">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -717,7 +729,7 @@
         <v>31</v>
       </c>
       <c r="D7">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E7">
         <v>22</v>
@@ -732,7 +744,7 @@
         <v>19</v>
       </c>
       <c r="I7">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -746,7 +758,7 @@
         <v>5</v>
       </c>
       <c r="D8">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E8">
         <v>23</v>
@@ -761,7 +773,7 @@
         <v>25</v>
       </c>
       <c r="I8">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -771,7 +783,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -801,40 +813,40 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>2236150003</v>
+        <v>2136110035</v>
       </c>
       <c r="B3" t="s">
         <v>20</v>
       </c>
       <c r="C3">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>2136110035</v>
+        <v>2136110029</v>
       </c>
       <c r="B4" t="s">
         <v>21</v>
       </c>
       <c r="C4">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5">
-        <v>2136110046</v>
+        <v>2236150003</v>
       </c>
       <c r="B5" t="s">
         <v>22</v>
       </c>
       <c r="C5">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6">
-        <v>2136110029</v>
+        <v>2136110046</v>
       </c>
       <c r="B6" t="s">
         <v>23</v>
@@ -851,34 +863,34 @@
         <v>24</v>
       </c>
       <c r="C7">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8">
-        <v>2136110002</v>
+        <v>2136110024</v>
       </c>
       <c r="B8" t="s">
         <v>25</v>
       </c>
       <c r="C8">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9">
-        <v>2136110024</v>
+        <v>2136110033</v>
       </c>
       <c r="B9" t="s">
         <v>26</v>
       </c>
       <c r="C9">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10">
-        <v>2136110033</v>
+        <v>2136110043</v>
       </c>
       <c r="B10" t="s">
         <v>27</v>
@@ -889,12 +901,45 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11">
-        <v>2136110032</v>
+        <v>2136110006</v>
       </c>
       <c r="B11" t="s">
         <v>28</v>
       </c>
       <c r="C11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12">
+        <v>2136110011</v>
+      </c>
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13">
+        <v>2136110002</v>
+      </c>
+      <c r="B13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14">
+        <v>2136110032</v>
+      </c>
+      <c r="B14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14">
         <v>4</v>
       </c>
     </row>
@@ -905,7 +950,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -927,29 +972,29 @@
         <v>2136110001</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C2">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>2136110030</v>
+        <v>2136110031</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C3">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>2136110016</v>
+        <v>2136110013</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C4">
         <v>6</v>
@@ -957,10 +1002,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5">
-        <v>2136110049</v>
+        <v>2136110008</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C5">
         <v>6</v>
@@ -968,10 +1013,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6">
-        <v>2136110031</v>
+        <v>2136110019</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C6">
         <v>6</v>
@@ -979,10 +1024,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7">
-        <v>2136110004</v>
+        <v>2136110030</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C7">
         <v>6</v>
@@ -990,32 +1035,32 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8">
-        <v>2136110022</v>
+        <v>2136110003</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C8">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9">
-        <v>2136110040</v>
+        <v>2136110021</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C9">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10">
-        <v>2136110021</v>
+        <v>2136110016</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C10">
         <v>5</v>
@@ -1023,10 +1068,10 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11">
-        <v>2136110019</v>
+        <v>2136110040</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C11">
         <v>5</v>
@@ -1034,10 +1079,10 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12">
-        <v>2136110047</v>
+        <v>2136110009</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C12">
         <v>5</v>
@@ -1045,65 +1090,65 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13">
-        <v>2136110048</v>
+        <v>2136110026</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C13">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14">
-        <v>2136110003</v>
+        <v>2136110022</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C14">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15">
-        <v>2136110010</v>
+        <v>2136110038</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C15">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16">
-        <v>2136110036</v>
+        <v>2136110047</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C16">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17">
-        <v>2136110038</v>
+        <v>2136110049</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C17">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18">
-        <v>2136110009</v>
+        <v>2136110036</v>
       </c>
       <c r="B18" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C18">
         <v>4</v>
@@ -1111,10 +1156,10 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19">
-        <v>2136110007</v>
+        <v>2136110010</v>
       </c>
       <c r="B19" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C19">
         <v>4</v>
@@ -1122,10 +1167,10 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20">
-        <v>2136110013</v>
+        <v>2136110004</v>
       </c>
       <c r="B20" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C20">
         <v>4</v>
@@ -1133,10 +1178,10 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21">
-        <v>2136110014</v>
+        <v>2136110007</v>
       </c>
       <c r="B21" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C21">
         <v>4</v>
@@ -1144,10 +1189,10 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22">
-        <v>2136110008</v>
+        <v>2136110045</v>
       </c>
       <c r="B22" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C22">
         <v>4</v>
@@ -1155,12 +1200,23 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23">
+        <v>2136110014</v>
+      </c>
+      <c r="B23" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24">
         <v>2136110020</v>
       </c>
-      <c r="B23" t="s">
-        <v>50</v>
-      </c>
-      <c r="C23">
+      <c r="B24" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24">
         <v>4</v>
       </c>
     </row>

</xml_diff>